<commit_message>
Update FSAR plot data with infilled spawning escapement time series
</commit_message>
<xml_diff>
--- a/FSAR 4-panel plot/FSAR_4-panel_data.xlsx
+++ b/FSAR 4-panel plot/FSAR_4-panel_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brownn\Documents\WCVI\C-68_WCVI_Chinook_work\FSAR 4-panel plot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brownn\Documents\WCVI\WCVI-CN-ResDoc\FSAR 4-panel plot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E9E698-E90F-42DF-890E-0AC8E9006A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4454888-0130-4134-9DD4-D28DBC5CFE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -397,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -424,10 +424,10 @@
         <v>1979</v>
       </c>
       <c r="B2">
-        <v>3408</v>
+        <v>4342.2344444444443</v>
       </c>
       <c r="D2">
-        <v>0.65523565010086182</v>
+        <v>0.62798842499999996</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -435,10 +435,10 @@
         <v>1980</v>
       </c>
       <c r="B3">
-        <v>7777.5</v>
+        <v>9873.3104952350241</v>
       </c>
       <c r="D3">
-        <v>0.66310583580613236</v>
+        <v>0.76827633399999995</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -446,10 +446,10 @@
         <v>1981</v>
       </c>
       <c r="B4">
-        <v>6635</v>
+        <v>7757.7920634920638</v>
       </c>
       <c r="D4">
-        <v>0.71285529715762275</v>
+        <v>0.73571767899999996</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -457,10 +457,10 @@
         <v>1982</v>
       </c>
       <c r="B5">
-        <v>7890</v>
+        <v>10201.78173185951</v>
       </c>
       <c r="D5">
-        <v>0.69820971867007653</v>
+        <v>0.65244785999999999</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -468,10 +468,10 @@
         <v>1983</v>
       </c>
       <c r="B6">
-        <v>3816</v>
+        <v>5661.329557713053</v>
       </c>
       <c r="D6">
-        <v>0.726003917727718</v>
+        <v>0.75765146500000002</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -479,10 +479,10 @@
         <v>1984</v>
       </c>
       <c r="B7">
-        <v>5470</v>
+        <v>7454.889411764706</v>
       </c>
       <c r="D7">
-        <v>0.63248638838475491</v>
+        <v>0.75568564999999999</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -490,13 +490,13 @@
         <v>1985</v>
       </c>
       <c r="B8">
-        <v>4599</v>
+        <v>6242.570323464136</v>
       </c>
       <c r="C8">
         <v>178052.85652432509</v>
       </c>
       <c r="D8">
-        <v>0.58500590318772139</v>
+        <v>0.67942554899999996</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -504,13 +504,13 @@
         <v>1986</v>
       </c>
       <c r="B9">
-        <v>4228</v>
+        <v>6343.3141752345346</v>
       </c>
       <c r="C9">
         <v>61106.378035804024</v>
       </c>
       <c r="D9">
-        <v>0.47697368421052622</v>
+        <v>0.64320170099999996</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -518,13 +518,13 @@
         <v>1987</v>
       </c>
       <c r="B10">
-        <v>3846</v>
+        <v>4381.2786665148406</v>
       </c>
       <c r="C10">
         <v>45762.702178710068</v>
       </c>
       <c r="D10">
-        <v>0.32962962962962961</v>
+        <v>0.26142261100000003</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -532,13 +532,13 @@
         <v>1988</v>
       </c>
       <c r="B11">
-        <v>7323.5</v>
+        <v>8304.1557164567494</v>
       </c>
       <c r="C11">
         <v>91527.209684412024</v>
       </c>
       <c r="D11">
-        <v>0.40537974683544298</v>
+        <v>0.34751590100000002</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -546,13 +546,13 @@
         <v>1989</v>
       </c>
       <c r="B12">
-        <v>8091</v>
+        <v>9538.8294966236954</v>
       </c>
       <c r="C12">
         <v>101042.00068755817</v>
       </c>
       <c r="D12">
-        <v>0.37232264924806308</v>
+        <v>0.28997511999999998</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -560,13 +560,13 @@
         <v>1990</v>
       </c>
       <c r="B13">
-        <v>6932</v>
+        <v>8246.9237875997551</v>
       </c>
       <c r="C13">
         <v>196190.27181940814</v>
       </c>
       <c r="D13">
-        <v>0.45970926058865752</v>
+        <v>0.34718398900000003</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -574,13 +574,13 @@
         <v>1991</v>
       </c>
       <c r="B14">
-        <v>8378</v>
+        <v>8648.7993462867216</v>
       </c>
       <c r="C14">
         <v>272793.05672136648</v>
       </c>
       <c r="D14">
-        <v>0.46826832621752668</v>
+        <v>0.49107056799999999</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -588,13 +588,13 @@
         <v>1992</v>
       </c>
       <c r="B15">
-        <v>9479</v>
+        <v>10161.952704403269</v>
       </c>
       <c r="C15">
         <v>509000.80816585355</v>
       </c>
       <c r="D15">
-        <v>0.63887909763835049</v>
+        <v>0.63934258300000002</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -602,13 +602,13 @@
         <v>1993</v>
       </c>
       <c r="B16">
-        <v>9998</v>
+        <v>11291.19643953346</v>
       </c>
       <c r="C16">
         <v>277035.93881388317</v>
       </c>
       <c r="D16">
-        <v>0.50544045312267105</v>
+        <v>0.59468891599999996</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -616,13 +616,13 @@
         <v>1994</v>
       </c>
       <c r="B17">
-        <v>7932</v>
+        <v>11938.563842848371</v>
       </c>
       <c r="C17">
         <v>177866.08154183425</v>
       </c>
       <c r="D17">
-        <v>0.49828450778569544</v>
+        <v>0.64058026199999996</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -630,13 +630,13 @@
         <v>1995</v>
       </c>
       <c r="B18">
-        <v>6205</v>
+        <v>6353</v>
       </c>
       <c r="C18">
         <v>42515.378397203545</v>
       </c>
       <c r="D18">
-        <v>0.31547220361687883</v>
+        <v>0.58439851300000001</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -644,13 +644,13 @@
         <v>1996</v>
       </c>
       <c r="B19">
-        <v>9847</v>
+        <v>10609</v>
       </c>
       <c r="C19">
         <v>29222.436046453673</v>
       </c>
       <c r="D19">
-        <v>0.21957040572792366</v>
+        <v>0.21791869699999999</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -658,13 +658,13 @@
         <v>1997</v>
       </c>
       <c r="B20">
-        <v>13051</v>
+        <v>14176</v>
       </c>
       <c r="C20">
         <v>83599.592797319347</v>
       </c>
       <c r="D20">
-        <v>0.36310329273793424</v>
+        <v>0.247923591</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -672,13 +672,13 @@
         <v>1998</v>
       </c>
       <c r="B21">
-        <v>22067</v>
+        <v>29840</v>
       </c>
       <c r="C21">
         <v>124815.11032298941</v>
       </c>
       <c r="D21">
-        <v>0.39156436890147944</v>
+        <v>0.37600623100000002</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -686,13 +686,13 @@
         <v>1999</v>
       </c>
       <c r="B22">
-        <v>16173</v>
+        <v>20847</v>
       </c>
       <c r="C22">
         <v>65090.186561109469</v>
       </c>
       <c r="D22">
-        <v>0.38380566801619431</v>
+        <v>0.563086753</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -700,13 +700,13 @@
         <v>2000</v>
       </c>
       <c r="B23">
-        <v>7582</v>
+        <v>8110</v>
       </c>
       <c r="C23">
         <v>9283.2749094746905</v>
       </c>
       <c r="D23">
-        <v>0.19634703196347034</v>
+        <v>0.38669400599999998</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -714,13 +714,13 @@
         <v>2001</v>
       </c>
       <c r="B24">
-        <v>7987</v>
+        <v>8565.2738095238092</v>
       </c>
       <c r="C24">
         <v>11749.098533839046</v>
       </c>
       <c r="D24">
-        <v>0.11752136752136753</v>
+        <v>7.0410851999999996E-2</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -728,13 +728,13 @@
         <v>2002</v>
       </c>
       <c r="B25">
-        <v>10939</v>
+        <v>22123</v>
       </c>
       <c r="C25">
         <v>61427.136870085698</v>
       </c>
       <c r="D25">
-        <v>0.27015355086372361</v>
+        <v>0.21321663399999999</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -742,13 +742,13 @@
         <v>2003</v>
       </c>
       <c r="B26">
-        <v>13178</v>
+        <v>26789</v>
       </c>
       <c r="C26">
         <v>81911.385482238082</v>
       </c>
       <c r="D26">
-        <v>0.27449664429530196</v>
+        <v>0.21493885400000001</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -756,13 +756,13 @@
         <v>2004</v>
       </c>
       <c r="B27">
-        <v>19800</v>
+        <v>23272</v>
       </c>
       <c r="C27">
         <v>143580.23948566156</v>
       </c>
       <c r="D27">
-        <v>0.35162396610853347</v>
+        <v>0.34575744400000002</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -770,13 +770,13 @@
         <v>2005</v>
       </c>
       <c r="B28">
-        <v>7762</v>
+        <v>8608.9995395948426</v>
       </c>
       <c r="C28">
         <v>103258.77184158686</v>
       </c>
       <c r="D28">
-        <v>0.39802736239261849</v>
+        <v>0.40466605100000003</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -784,13 +784,13 @@
         <v>2006</v>
       </c>
       <c r="B29">
-        <v>14119</v>
+        <v>13582.08695652174</v>
       </c>
       <c r="C29">
         <v>90916.999103899143</v>
       </c>
       <c r="D29">
-        <v>0.31541725601131543</v>
+        <v>0.34295819999999999</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -798,13 +798,13 @@
         <v>2007</v>
       </c>
       <c r="B30">
-        <v>8524</v>
+        <v>7977.826086956522</v>
       </c>
       <c r="C30">
         <v>92774.171285073113</v>
       </c>
       <c r="D30">
-        <v>0.43442265795206969</v>
+        <v>0.44592135100000002</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -812,13 +812,13 @@
         <v>2008</v>
       </c>
       <c r="B31">
-        <v>8309</v>
+        <v>6683</v>
       </c>
       <c r="C31">
         <v>31922.274973775915</v>
       </c>
       <c r="D31">
-        <v>0.24534161490683229</v>
+        <v>0.35146423500000001</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -826,13 +826,13 @@
         <v>2009</v>
       </c>
       <c r="B32">
-        <v>11694</v>
+        <v>13856.95652173913</v>
       </c>
       <c r="C32">
         <v>72462.402256321846</v>
       </c>
       <c r="D32">
-        <v>0.44186046511627908</v>
+        <v>0.48343202800000001</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -840,13 +840,13 @@
         <v>2010</v>
       </c>
       <c r="B33">
-        <v>11257</v>
+        <v>10932</v>
       </c>
       <c r="C33">
         <v>40984.53283981343</v>
       </c>
       <c r="D33">
-        <v>0.3023082650781832</v>
+        <v>0.30033380500000001</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -854,13 +854,13 @@
         <v>2011</v>
       </c>
       <c r="B34">
-        <v>10344</v>
+        <v>11295</v>
       </c>
       <c r="C34">
         <v>92469.933435721759</v>
       </c>
       <c r="D34">
-        <v>0.36902242911553118</v>
+        <v>0.34518059099999998</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -868,13 +868,13 @@
         <v>2012</v>
       </c>
       <c r="B35">
-        <v>8920</v>
+        <v>8652.9524375743167</v>
       </c>
       <c r="C35">
         <v>41653.449926746223</v>
       </c>
       <c r="D35">
-        <v>0.33998005982053842</v>
+        <v>0.43071284199999998</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -882,13 +882,13 @@
         <v>2013</v>
       </c>
       <c r="B36">
-        <v>16753</v>
+        <v>17803</v>
       </c>
       <c r="C36">
         <v>87812.369036630058</v>
       </c>
       <c r="D36">
-        <v>0.33356741573033716</v>
+        <v>0.32861700599999999</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -896,13 +896,13 @@
         <v>2014</v>
       </c>
       <c r="B37">
-        <v>10560</v>
+        <v>13288</v>
       </c>
       <c r="C37">
         <v>69557.409547255767</v>
       </c>
       <c r="D37">
-        <v>0.37658495350803034</v>
+        <v>0.44020615299999999</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -910,13 +910,13 @@
         <v>2015</v>
       </c>
       <c r="B38">
-        <v>22247</v>
+        <v>23619.470868014268</v>
       </c>
       <c r="C38">
         <v>87019.245961369161</v>
       </c>
       <c r="D38">
-        <v>0.29635949943117185</v>
+        <v>0.25517959899999998</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -924,13 +924,13 @@
         <v>2016</v>
       </c>
       <c r="B39">
-        <v>21637</v>
+        <v>23162</v>
       </c>
       <c r="C39">
         <v>130058.17072369857</v>
       </c>
       <c r="D39">
-        <v>0.42109242109242118</v>
+        <v>0.38341636899999998</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -938,13 +938,13 @@
         <v>2017</v>
       </c>
       <c r="B40">
-        <v>16776</v>
+        <v>18250</v>
       </c>
       <c r="C40">
         <v>113806.20961372726</v>
       </c>
       <c r="D40">
-        <v>0.36816326530612253</v>
+        <v>0.43962685099999999</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -952,13 +952,13 @@
         <v>2018</v>
       </c>
       <c r="B41">
-        <v>11861</v>
+        <v>13737</v>
       </c>
       <c r="C41">
         <v>93631.047296952456</v>
       </c>
       <c r="D41">
-        <v>0.34166111481234734</v>
+        <v>0.30269774599999999</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -966,13 +966,13 @@
         <v>2019</v>
       </c>
       <c r="B42">
-        <v>14875</v>
+        <v>16721.621375781691</v>
       </c>
       <c r="C42">
         <v>100071.49063461184</v>
       </c>
       <c r="D42">
-        <v>0.33363101882860752</v>
+        <v>0.36600726700000003</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -980,13 +980,13 @@
         <v>2020</v>
       </c>
       <c r="B43">
-        <v>12003</v>
+        <v>20125</v>
       </c>
       <c r="C43">
         <v>68648.098394354951</v>
       </c>
       <c r="D43">
-        <v>0.2419210053859964</v>
+        <v>0.28084114100000002</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -994,13 +994,13 @@
         <v>2021</v>
       </c>
       <c r="B44">
-        <v>15604</v>
+        <v>21689</v>
       </c>
       <c r="C44">
         <v>90895.461868662154</v>
       </c>
       <c r="D44">
-        <v>0.28387850467289721</v>
+        <v>0.31995095899999998</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1008,13 +1008,27 @@
         <v>2022</v>
       </c>
       <c r="B45">
-        <v>10424</v>
+        <v>18243</v>
       </c>
       <c r="C45">
-        <v>160366.52429505222</v>
+        <v>160604.8106129762</v>
       </c>
       <c r="D45">
-        <v>0.39356017997750287</v>
+        <v>0.40610734500000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>2023</v>
+      </c>
+      <c r="B46">
+        <v>33612.247299602037</v>
+      </c>
+      <c r="C46">
+        <v>83986.667958935839</v>
+      </c>
+      <c r="D46">
+        <v>0.234145889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>